<commit_message>
changes for unigram and bigram
</commit_message>
<xml_diff>
--- a/resources/Answers for University PDF2.xlsx
+++ b/resources/Answers for University PDF2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FYP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FYP\Evaluation Excel\University2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{43CDE942-F1DE-4DAF-AE72-A00AA604DD80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B7BFCA-3E8D-4B65-8687-7DE2649A342D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{CE26CBB1-E2C9-4607-A141-BC648DFA268C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="78">
   <si>
     <t>The Faculty of Information Technology is the youngest of the three faculties of the University of Moratuwa.</t>
   </si>
@@ -203,30 +203,6 @@
     <t>The main responsibility of the Undergraduate Studies Division within the Faculty is to handle matters pertaining to the academic affairs of the undergraduate study programmes of the Faculty, including students' attendance monitoring and student feedback administration.</t>
   </si>
   <si>
-    <t>The Faculty of Information Technology (FOIT) at the University of Moratuwa is a relatively new department within the national university system of Sri Lanka, established in June 2001. Its primary objective is to increase the number of IT professionals in the country by at least another 500. The faculty offers two internal degree programs, B.Sc. (Hons.) in Information Technology and B.Sc. (Hons.) in Information Technology &amp; Management, as well as an external degree program, Bachelor of Information Technology. The faculty also conducts postgraduate programs such as Master of Science in Information Technology, Masters of Science in Artificial Intelligence, Master of Philosophy, and Doctoral degrees. There are currently about 600 undergraduate students studying at the faculty, which is managed by three departments: Department of Information Technology, Department of Computational Mathematics, and Department of Interdisciplinary Studies. For administrative purposes, the faculty has two divisions: the Undergraduate Studies Division and the Postgraduate Studies Division.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The primary objective of the Faculty of Information Technology (FOIT) at the University of Moratuwa is to increase the number of IT professionals in Sri Lanka by at least another 500. </t>
-  </si>
-  <si>
-    <t>The primary objectives of the Faculty of Information Technology (FOIT) at the University of Moratuwa are to increase the number of IT professionals in Sri Lanka by at least another 500, the introduction of postgraduate programmes, carrying out research programmes for the industry in order to solve technical problems, providing consultancies to the local industry and creating an educational environment for the continuous professional development of IT professionals in Sri Lank a.</t>
-  </si>
-  <si>
-    <t>The primary objective of the FOIT at the University of Moratuwa is to increase the number of IT professionals in Sri Lanka by at least another 500.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The main objectives of the Faculty of Information Technology (FOIT) at the University of Moratuwa include increasing the number of IT professionals in Sri Lanka by at least another 500, introducing postgraduate programmes, carrying out research programmes for the industry to solve technical problems, providing consultancies to the local industry and creating an educational environment for the continuous professional development of IT professionals in Sri Lanka. </t>
-  </si>
-  <si>
-    <t>The primary objective of the Faculty of Information Technology (FOIT) at the University of Moratuwa is to increase the number of IT professionals in Sri Lanka by at least another 500.</t>
-  </si>
-  <si>
-    <t>The main objectives of the Faculty of Information Technology (FOIT) at the University of Moratuwa include increasing the number of IT professionals in Sri Lanka by at least another 500, introducing postgraduate programmes, carrying out research programmes for the industry in order to solve technical problems, providing consultancies to the local industry and creating an educational environment for the continuous professional development of IT professionals in Sri Lank a.</t>
-  </si>
-  <si>
-    <t>The main objectives of the Faculty of Information Technology (FOIT) at the University of Moratuwa are to increase the number of IT professionals in Sri Lanka by at least another 500, to introduce postgraduate programmes, to carry out research programmes for the industry in order to solve technical problems, to provide consultancies to the local industry, to create an educational environment for the continuous professional development of IT professionals in Sri Lank a and to become an entity which both the students and the industry would look up to.</t>
-  </si>
-  <si>
     <t>The Faculty of Information Technology aims to contribute to the local IT industry by increasing the number of IT professionals, introducing postgraduate programmes, carrying out research programmes for the industry, providing consultancies to the local industry and creating an educational environment for the continuous professional development of IT professionals.</t>
   </si>
   <si>
@@ -255,6 +231,45 @@
   </si>
   <si>
     <t>The Faculty of Information Technology contributes to the local IT industry in several ways. First, it increases the number of IT professionals in the country by at least another 500 through its internal and external degree programmes. Second, it provides consultancies to the local industry to solve technical problems. Third, it carries out research programmes for the industry to address technical issues. Fourth, it designs professional development programmes to meet the immediate needs of the local IT industry. Finally, it collaborates with other departments to offer relevant subjects for degree programmes and handles matters pertaining to academic affairs of undergraduate and postgraduate programmes through its divisions.</t>
+  </si>
+  <si>
+    <t>Nine batches have already passed out after completing their studies.</t>
+  </si>
+  <si>
+    <t>The Faculty of Information Technology at the University of Moratuwa is conducting Master of Science in Information Technology, Masters of Science in Artificial Intelligence, Master of Philosophy and Doctoral degrees as postgraduate programmes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Postgraduate Studies Division of the Faculty of Information Technology contributes to the faculty by handling matters pertaining to taught postgraduate programmes and research degrees. It oversees the academic affairs of these programmes, including student attendance monitoring and student feedback administration. </t>
+  </si>
+  <si>
+    <t>The Postgraduate Studies Division contributes to the Faculty of Information Technology by handling matters pertaining to taught postgraduate programmes and research degrees. This includes monitoring student progress, administering student feedback, and ensuring that students receive a high-quality education in their chosen fields of study. Additionally, the Postgraduate Studies Division collaborates with industry partners to develop new postgraduate programmes and research opportunities, which helps to keep the Faculty at the forefront of technological innovation and development. Overall, the Postgraduate Studies Division plays a crucial role in advancing knowledge and skills within the IT industry and preparing students for successful careers in this rapidly growing field.</t>
+  </si>
+  <si>
+    <t>The Postgraduate Studies Division is responsible for handling matters pertaining to taught postgraduate programmes and research degrees for the Faculty of Information Technology. This includes administering student attendance, feedback and related academic activities for these programmes. Additionally, the division also collaborates with other departments in the faculty to offer relevant subjects for these programmes.</t>
+  </si>
+  <si>
+    <t>The Postgraduate Studies Division is responsible for handling matters pertaining to taught postgraduate programmes and research degrees.</t>
+  </si>
+  <si>
+    <t>The Postgraduate Studies Division plays a crucial role in advancing knowledge and skills within the IT industry by offering various postgraduate programmes such as Master of Science in Information Technology, Masters of Science in Artificial Intelligence, Master of Philosophy and Doctoral degrees. These programmes are designed to meet the immediate needs of the local IT industry and provide opportunities for professionals to enhance their skills and knowledge. The Division also carries out research programmes for the industry to solve technical problems and provides consultancies to local businesses. Overall, the Postgraduate Studies Division plays a significant role in advancing knowledge and skills within the IT industry by offering high-quality education and research opportunities to professionals.</t>
+  </si>
+  <si>
+    <t>The Postgraduate Studies Division of the Faculty of Information Technology offers three postgraduate programmes, namely Master of Science in Information Technology, Masters of Science in Artificial Intelligence and Master of Philosophy.</t>
+  </si>
+  <si>
+    <t>The Postgraduate Studies Division is responsible for handling matters pertaining to taught postgraduate programmes and research degrees of the Faculty of Information Technology.</t>
+  </si>
+  <si>
+    <t>Each department is managed by the respective Head of Department.</t>
+  </si>
+  <si>
+    <t>The question does not provide enough context to determine the names of the people who manage each department in the faculty.</t>
+  </si>
+  <si>
+    <t>The names of the individuals who manage each department in the faculty are not mentioned in the given context, only their roles are described.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The heads of the departments in the Faculty of Information Technology are Dr. Chandana Wickramasinghe (Department of Information Technology), Dr. Tilak Rambukwella (Department of Computational Mathematics), and Dr. Anura Fernando (Department of Interdisciplinary Studies). </t>
   </si>
 </sst>
 </file>
@@ -647,15 +662,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B19A0F9-8CDE-4BF8-998E-8C17FD0D4EC7}">
-  <dimension ref="A1:A100"/>
+  <dimension ref="A1:A103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91:XFD91"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="180" customWidth="1"/>
+    <col min="1" max="1" width="180" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -1069,93 +1085,108 @@
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>56</v>
+      <c r="A83" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
-        <v>57</v>
+      <c r="A84" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
-        <v>62</v>
+      <c r="A90" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="3" t="s">
-        <v>65</v>
+      <c r="A93" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="3" t="s">
-        <v>66</v>
+      <c r="A94" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="2" t="s">
-        <v>72</v>
+      <c r="A100" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>